<commit_message>
separate admin field data
</commit_message>
<xml_diff>
--- a/newdata.xlsx
+++ b/newdata.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA19"/>
+  <dimension ref="A1:AA23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,7 +415,7 @@
         <v>URL</v>
       </c>
       <c r="B2" t="str">
-        <v>https://preprod-binary.epixel.link/en/customer-register/</v>
+        <v>https://prod-unilevel.epixel.link/en/register/</v>
       </c>
     </row>
     <row r="3">
@@ -423,7 +423,7 @@
         <v>Sponsor</v>
       </c>
       <c r="B3" t="str">
-        <v>release-mpfp-binary-business-admin</v>
+        <v>mpfp-base-unilevel-business-admin,user1,user2</v>
       </c>
     </row>
     <row r="4">
@@ -450,7 +450,10 @@
         <v>Subdomain</v>
       </c>
       <c r="B6" t="str">
-        <v>onetest12</v>
+        <v>antp087123</v>
+      </c>
+      <c r="C6" t="str">
+        <v>If needed change</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +493,7 @@
         <v>Enrollment Package</v>
       </c>
       <c r="B11" t="str">
-        <v>enrollment-package-9</v>
+        <v>Bronze</v>
       </c>
       <c r="C11" t="str">
         <v/>
@@ -504,89 +507,89 @@
         <v>click</v>
       </c>
     </row>
-    <row r="19">
-      <c r="B19" t="str">
-        <v/>
-      </c>
-      <c r="C19" t="str">
-        <v/>
-      </c>
-      <c r="D19" t="str">
-        <v/>
-      </c>
-      <c r="E19" t="str">
-        <v/>
-      </c>
-      <c r="F19" t="str">
-        <v/>
-      </c>
-      <c r="G19" t="str">
-        <v/>
-      </c>
-      <c r="H19" t="str">
-        <v/>
-      </c>
-      <c r="I19" t="str">
-        <v/>
-      </c>
-      <c r="J19" t="str">
-        <v/>
-      </c>
-      <c r="K19" t="str">
-        <v/>
-      </c>
-      <c r="L19" t="str">
-        <v/>
-      </c>
-      <c r="M19" t="str">
-        <v/>
-      </c>
-      <c r="N19" t="str">
-        <v/>
-      </c>
-      <c r="O19" t="str">
-        <v/>
-      </c>
-      <c r="P19" t="str">
-        <v/>
-      </c>
-      <c r="Q19" t="str">
-        <v/>
-      </c>
-      <c r="R19" t="str">
-        <v/>
-      </c>
-      <c r="S19" t="str">
-        <v/>
-      </c>
-      <c r="T19" t="str">
-        <v/>
-      </c>
-      <c r="U19" t="str">
-        <v/>
-      </c>
-      <c r="V19" t="str">
-        <v/>
-      </c>
-      <c r="W19" t="str">
-        <v/>
-      </c>
-      <c r="X19" t="str">
-        <v/>
-      </c>
-      <c r="Y19" t="str">
-        <v/>
-      </c>
-      <c r="Z19" t="str">
-        <v/>
-      </c>
-      <c r="AA19" t="str">
+    <row r="23">
+      <c r="B23" t="str">
+        <v/>
+      </c>
+      <c r="C23" t="str">
+        <v/>
+      </c>
+      <c r="D23" t="str">
+        <v/>
+      </c>
+      <c r="E23" t="str">
+        <v/>
+      </c>
+      <c r="F23" t="str">
+        <v/>
+      </c>
+      <c r="G23" t="str">
+        <v/>
+      </c>
+      <c r="H23" t="str">
+        <v/>
+      </c>
+      <c r="I23" t="str">
+        <v/>
+      </c>
+      <c r="J23" t="str">
+        <v/>
+      </c>
+      <c r="K23" t="str">
+        <v/>
+      </c>
+      <c r="L23" t="str">
+        <v/>
+      </c>
+      <c r="M23" t="str">
+        <v/>
+      </c>
+      <c r="N23" t="str">
+        <v/>
+      </c>
+      <c r="O23" t="str">
+        <v/>
+      </c>
+      <c r="P23" t="str">
+        <v/>
+      </c>
+      <c r="Q23" t="str">
+        <v/>
+      </c>
+      <c r="R23" t="str">
+        <v/>
+      </c>
+      <c r="S23" t="str">
+        <v/>
+      </c>
+      <c r="T23" t="str">
+        <v/>
+      </c>
+      <c r="U23" t="str">
+        <v/>
+      </c>
+      <c r="V23" t="str">
+        <v/>
+      </c>
+      <c r="W23" t="str">
+        <v/>
+      </c>
+      <c r="X23" t="str">
+        <v/>
+      </c>
+      <c r="Y23" t="str">
+        <v/>
+      </c>
+      <c r="Z23" t="str">
+        <v/>
+      </c>
+      <c r="AA23" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AA19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AA23"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
separate comm with sponsor
</commit_message>
<xml_diff>
--- a/newdata.xlsx
+++ b/newdata.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA19"/>
+  <dimension ref="A1:AA23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,7 +415,7 @@
         <v>URL</v>
       </c>
       <c r="B2" t="str">
-        <v>https://preprod-binary.epixel.link/en/customer-register/</v>
+        <v>https://prod-unilevel.epixel.link/en/register/</v>
       </c>
     </row>
     <row r="3">
@@ -423,7 +423,7 @@
         <v>Sponsor</v>
       </c>
       <c r="B3" t="str">
-        <v>release-mpfp-binary-business-admin</v>
+        <v>mpfp-base-unilevel-business-admin,user1,user2</v>
       </c>
     </row>
     <row r="4">
@@ -450,7 +450,10 @@
         <v>Subdomain</v>
       </c>
       <c r="B6" t="str">
-        <v>onete123</v>
+        <v>antp087123</v>
+      </c>
+      <c r="C6" t="str">
+        <v>If needed change</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +493,7 @@
         <v>Enrollment Package</v>
       </c>
       <c r="B11" t="str">
-        <v>enrollment-package-9</v>
+        <v>Bronze</v>
       </c>
       <c r="C11" t="str">
         <v/>
@@ -504,89 +507,89 @@
         <v>click</v>
       </c>
     </row>
-    <row r="19">
-      <c r="B19" t="str">
-        <v/>
-      </c>
-      <c r="C19" t="str">
-        <v/>
-      </c>
-      <c r="D19" t="str">
-        <v/>
-      </c>
-      <c r="E19" t="str">
-        <v/>
-      </c>
-      <c r="F19" t="str">
-        <v/>
-      </c>
-      <c r="G19" t="str">
-        <v/>
-      </c>
-      <c r="H19" t="str">
-        <v/>
-      </c>
-      <c r="I19" t="str">
-        <v/>
-      </c>
-      <c r="J19" t="str">
-        <v/>
-      </c>
-      <c r="K19" t="str">
-        <v/>
-      </c>
-      <c r="L19" t="str">
-        <v/>
-      </c>
-      <c r="M19" t="str">
-        <v/>
-      </c>
-      <c r="N19" t="str">
-        <v/>
-      </c>
-      <c r="O19" t="str">
-        <v/>
-      </c>
-      <c r="P19" t="str">
-        <v/>
-      </c>
-      <c r="Q19" t="str">
-        <v/>
-      </c>
-      <c r="R19" t="str">
-        <v/>
-      </c>
-      <c r="S19" t="str">
-        <v/>
-      </c>
-      <c r="T19" t="str">
-        <v/>
-      </c>
-      <c r="U19" t="str">
-        <v/>
-      </c>
-      <c r="V19" t="str">
-        <v/>
-      </c>
-      <c r="W19" t="str">
-        <v/>
-      </c>
-      <c r="X19" t="str">
-        <v/>
-      </c>
-      <c r="Y19" t="str">
-        <v/>
-      </c>
-      <c r="Z19" t="str">
-        <v/>
-      </c>
-      <c r="AA19" t="str">
+    <row r="23">
+      <c r="B23" t="str">
+        <v/>
+      </c>
+      <c r="C23" t="str">
+        <v/>
+      </c>
+      <c r="D23" t="str">
+        <v/>
+      </c>
+      <c r="E23" t="str">
+        <v/>
+      </c>
+      <c r="F23" t="str">
+        <v/>
+      </c>
+      <c r="G23" t="str">
+        <v/>
+      </c>
+      <c r="H23" t="str">
+        <v/>
+      </c>
+      <c r="I23" t="str">
+        <v/>
+      </c>
+      <c r="J23" t="str">
+        <v/>
+      </c>
+      <c r="K23" t="str">
+        <v/>
+      </c>
+      <c r="L23" t="str">
+        <v/>
+      </c>
+      <c r="M23" t="str">
+        <v/>
+      </c>
+      <c r="N23" t="str">
+        <v/>
+      </c>
+      <c r="O23" t="str">
+        <v/>
+      </c>
+      <c r="P23" t="str">
+        <v/>
+      </c>
+      <c r="Q23" t="str">
+        <v/>
+      </c>
+      <c r="R23" t="str">
+        <v/>
+      </c>
+      <c r="S23" t="str">
+        <v/>
+      </c>
+      <c r="T23" t="str">
+        <v/>
+      </c>
+      <c r="U23" t="str">
+        <v/>
+      </c>
+      <c r="V23" t="str">
+        <v/>
+      </c>
+      <c r="W23" t="str">
+        <v/>
+      </c>
+      <c r="X23" t="str">
+        <v/>
+      </c>
+      <c r="Y23" t="str">
+        <v/>
+      </c>
+      <c r="Z23" t="str">
+        <v/>
+      </c>
+      <c r="AA23" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AA19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AA23"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
stripe payment case and delever address page
</commit_message>
<xml_diff>
--- a/newdata.xlsx
+++ b/newdata.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA23"/>
+  <dimension ref="A1:AA24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,7 +423,7 @@
         <v>Sponsor</v>
       </c>
       <c r="B3" t="str">
-        <v>mpfp-base-unilevel-business-admin,user1,user2</v>
+        <v>mpfp-base-unilevel-business-admin</v>
       </c>
     </row>
     <row r="4">
@@ -445,28 +445,20 @@
         <v/>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Subdomain</v>
-      </c>
-      <c r="B6" t="str">
-        <v>antp087123</v>
-      </c>
-      <c r="C6" t="str">
-        <v>If needed change</v>
-      </c>
-    </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Password</v>
+        <v>Subdomain</v>
       </c>
       <c r="B7" t="str">
-        <v>As@12345</v>
+        <v>rootcase20</v>
+      </c>
+      <c r="C7" t="str">
+        <v>If needed change</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Password Confirm</v>
+        <v>Password</v>
       </c>
       <c r="B8" t="str">
         <v>As@12345</v>
@@ -474,15 +466,15 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Terms and Conditions</v>
+        <v>Password Confirm</v>
       </c>
       <c r="B9" t="str">
-        <v>click</v>
+        <v>As@12345</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>addnew-member</v>
+        <v>Terms and Conditions</v>
       </c>
       <c r="B10" t="str">
         <v>click</v>
@@ -490,106 +482,114 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Enrollment Package</v>
+        <v>addnew-member</v>
       </c>
       <c r="B11" t="str">
-        <v>Bronze</v>
-      </c>
-      <c r="C11" t="str">
-        <v/>
+        <v>click</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
+        <v>Enrollment Package</v>
+      </c>
+      <c r="B12" t="str">
+        <v>enrollment-package-9</v>
+      </c>
+      <c r="C12" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
         <v>Proceed</v>
       </c>
-      <c r="B12" t="str">
+      <c r="B13" t="str">
         <v>click</v>
       </c>
     </row>
-    <row r="23">
-      <c r="B23" t="str">
-        <v/>
-      </c>
-      <c r="C23" t="str">
-        <v/>
-      </c>
-      <c r="D23" t="str">
-        <v/>
-      </c>
-      <c r="E23" t="str">
-        <v/>
-      </c>
-      <c r="F23" t="str">
-        <v/>
-      </c>
-      <c r="G23" t="str">
-        <v/>
-      </c>
-      <c r="H23" t="str">
-        <v/>
-      </c>
-      <c r="I23" t="str">
-        <v/>
-      </c>
-      <c r="J23" t="str">
-        <v/>
-      </c>
-      <c r="K23" t="str">
-        <v/>
-      </c>
-      <c r="L23" t="str">
-        <v/>
-      </c>
-      <c r="M23" t="str">
-        <v/>
-      </c>
-      <c r="N23" t="str">
-        <v/>
-      </c>
-      <c r="O23" t="str">
-        <v/>
-      </c>
-      <c r="P23" t="str">
-        <v/>
-      </c>
-      <c r="Q23" t="str">
-        <v/>
-      </c>
-      <c r="R23" t="str">
-        <v/>
-      </c>
-      <c r="S23" t="str">
-        <v/>
-      </c>
-      <c r="T23" t="str">
-        <v/>
-      </c>
-      <c r="U23" t="str">
-        <v/>
-      </c>
-      <c r="V23" t="str">
-        <v/>
-      </c>
-      <c r="W23" t="str">
-        <v/>
-      </c>
-      <c r="X23" t="str">
-        <v/>
-      </c>
-      <c r="Y23" t="str">
-        <v/>
-      </c>
-      <c r="Z23" t="str">
-        <v/>
-      </c>
-      <c r="AA23" t="str">
+    <row r="24">
+      <c r="B24" t="str">
+        <v/>
+      </c>
+      <c r="C24" t="str">
+        <v/>
+      </c>
+      <c r="D24" t="str">
+        <v/>
+      </c>
+      <c r="E24" t="str">
+        <v/>
+      </c>
+      <c r="F24" t="str">
+        <v/>
+      </c>
+      <c r="G24" t="str">
+        <v/>
+      </c>
+      <c r="H24" t="str">
+        <v/>
+      </c>
+      <c r="I24" t="str">
+        <v/>
+      </c>
+      <c r="J24" t="str">
+        <v/>
+      </c>
+      <c r="K24" t="str">
+        <v/>
+      </c>
+      <c r="L24" t="str">
+        <v/>
+      </c>
+      <c r="M24" t="str">
+        <v/>
+      </c>
+      <c r="N24" t="str">
+        <v/>
+      </c>
+      <c r="O24" t="str">
+        <v/>
+      </c>
+      <c r="P24" t="str">
+        <v/>
+      </c>
+      <c r="Q24" t="str">
+        <v/>
+      </c>
+      <c r="R24" t="str">
+        <v/>
+      </c>
+      <c r="S24" t="str">
+        <v/>
+      </c>
+      <c r="T24" t="str">
+        <v/>
+      </c>
+      <c r="U24" t="str">
+        <v/>
+      </c>
+      <c r="V24" t="str">
+        <v/>
+      </c>
+      <c r="W24" t="str">
+        <v/>
+      </c>
+      <c r="X24" t="str">
+        <v/>
+      </c>
+      <c r="Y24" t="str">
+        <v/>
+      </c>
+      <c r="Z24" t="str">
+        <v/>
+      </c>
+      <c r="AA24" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AA23"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AA24"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>